<commit_message>
Commit 2019-04-18 kl. 17:36
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Administration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14163B52-FB46-43AD-91CF-F43D213261E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4202FBA1-0522-465F-AA50-9A4CA57A7B56}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -691,19 +685,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D783D0-5715-48A8-A723-8C2ABC65314E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -751,10 +743,10 @@
       <c r="H3" s="13"/>
       <c r="J3" s="10">
         <f>125-K3</f>
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K3" s="10">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
@@ -772,9 +764,9 @@
         <v>16</v>
       </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 2019-05-03 kl. 17:30
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -685,7 +685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -743,10 +743,10 @@
       <c r="H3" s="13"/>
       <c r="J3" s="10">
         <f>125-K3</f>
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K3" s="10">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
@@ -774,19 +774,19 @@
         <v>17</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" s="19">
         <v>18</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 2019-05-08 kl. 09:28
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Week</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Days left</t>
+  </si>
+  <si>
+    <t>Total days</t>
   </si>
 </sst>
 </file>
@@ -92,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -220,57 +223,81 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -281,53 +308,32 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -336,26 +342,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -371,9 +371,24 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -693,21 +708,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:K28"/>
+  <dimension ref="C1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6.7109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
     <col min="4" max="8" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="21" t="s">
+    <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -725,281 +741,324 @@
       <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="18">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="12">
         <v>14</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="J3" s="10">
-        <f>125-K3</f>
-        <v>103</v>
-      </c>
-      <c r="K3" s="10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C4" s="19">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25">
+        <v>5</v>
+      </c>
+      <c r="K3" s="7">
+        <f>125-L3</f>
+        <v>101</v>
+      </c>
+      <c r="L3" s="7">
+        <f>SUM(I3:I28)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="13">
         <v>15</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="19">
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="13">
         <v>16</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C6" s="19">
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="13">
         <v>17</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="19">
+      <c r="D6" s="9"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="13">
         <v>18</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="19">
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="13">
         <v>19</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="19">
+      <c r="H8" s="20"/>
+      <c r="I8" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="13">
         <v>20</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="19">
+      <c r="H9" s="20"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="13">
         <v>21</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="19">
+      <c r="H10" s="20"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" s="13">
         <v>22</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="19">
+      <c r="H11" s="20"/>
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="13">
         <v>23</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="19">
+      <c r="H12" s="20"/>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="13">
         <v>24</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="19">
+      <c r="H13" s="20"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="13">
         <v>25</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="19">
+      <c r="H14" s="20"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="13">
         <v>26</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="19">
+      <c r="H15" s="20"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="13">
         <v>27</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="19">
+      <c r="H16" s="20"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="13">
         <v>28</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="19">
+      <c r="H17" s="20"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="13">
         <v>29</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="19">
+      <c r="H18" s="20"/>
+      <c r="I18" s="26"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="13">
         <v>30</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="19">
+      <c r="H19" s="20"/>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="13">
         <v>31</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="19">
+      <c r="H20" s="20"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="13">
         <v>32</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="19">
+      <c r="H21" s="20"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="13">
         <v>33</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="19">
+      <c r="H22" s="20"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="13">
         <v>34</v>
       </c>
-      <c r="D23" s="14"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="19">
+      <c r="H23" s="20"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="13">
         <v>35</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="19">
+      <c r="H24" s="20"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="13">
         <v>36</v>
       </c>
-      <c r="D25" s="14"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="19">
+      <c r="H25" s="20"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="13">
         <v>37</v>
       </c>
-      <c r="D26" s="14"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="19">
+      <c r="H26" s="20"/>
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="13">
         <v>38</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="20">
+      <c r="H27" s="20"/>
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="14">
         <v>39</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 2019-05-09 kl. 17:36
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -700,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -765,11 +765,11 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
@@ -830,11 +830,11 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="20"/>
       <c r="I8" s="26">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 2019-05-10 kl. 17:38
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Week</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>Total days</t>
+  </si>
+  <si>
+    <t>Maj</t>
+  </si>
+  <si>
+    <t>Juni</t>
+  </si>
+  <si>
+    <t>Juli</t>
+  </si>
+  <si>
+    <t>Augisti</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Date Friday</t>
   </si>
 </sst>
 </file>
@@ -342,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -387,6 +405,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -700,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -710,13 +732,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
     <col min="4" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
@@ -765,11 +790,11 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
@@ -823,6 +848,9 @@
       <c r="I7" s="26">
         <v>5</v>
       </c>
+      <c r="K7" s="28" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" s="13">
@@ -832,9 +860,15 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-      <c r="H8" s="20"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="26">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="11">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
@@ -847,6 +881,10 @@
       <c r="G9" s="1"/>
       <c r="H9" s="20"/>
       <c r="I9" s="26"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="11">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="13">
@@ -858,6 +896,10 @@
       <c r="G10" s="1"/>
       <c r="H10" s="20"/>
       <c r="I10" s="26"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="11">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="13">
@@ -869,6 +911,10 @@
       <c r="G11" s="1"/>
       <c r="H11" s="20"/>
       <c r="I11" s="26"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="11">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="13">
@@ -880,6 +926,12 @@
       <c r="G12" s="1"/>
       <c r="H12" s="20"/>
       <c r="I12" s="26"/>
+      <c r="J12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="11">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="13">
@@ -891,6 +943,10 @@
       <c r="G13" s="1"/>
       <c r="H13" s="20"/>
       <c r="I13" s="26"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="11">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="13">
@@ -902,6 +958,10 @@
       <c r="G14" s="1"/>
       <c r="H14" s="20"/>
       <c r="I14" s="26"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="11">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="13">
@@ -913,6 +973,10 @@
       <c r="G15" s="1"/>
       <c r="H15" s="20"/>
       <c r="I15" s="26"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="11">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="13">
@@ -924,8 +988,14 @@
       <c r="G16" s="1"/>
       <c r="H16" s="20"/>
       <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C17" s="13">
         <v>28</v>
       </c>
@@ -935,8 +1005,12 @@
       <c r="G17" s="1"/>
       <c r="H17" s="20"/>
       <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="29"/>
+      <c r="K17" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="13">
         <v>29</v>
       </c>
@@ -946,8 +1020,12 @@
       <c r="G18" s="1"/>
       <c r="H18" s="20"/>
       <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="29"/>
+      <c r="K18" s="11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="13">
         <v>30</v>
       </c>
@@ -957,8 +1035,12 @@
       <c r="G19" s="1"/>
       <c r="H19" s="20"/>
       <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="29"/>
+      <c r="K19" s="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="13">
         <v>31</v>
       </c>
@@ -968,8 +1050,14 @@
       <c r="G20" s="1"/>
       <c r="H20" s="20"/>
       <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21" s="13">
         <v>32</v>
       </c>
@@ -979,8 +1067,12 @@
       <c r="G21" s="1"/>
       <c r="H21" s="20"/>
       <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="29"/>
+      <c r="K21" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22" s="13">
         <v>33</v>
       </c>
@@ -990,8 +1082,12 @@
       <c r="G22" s="1"/>
       <c r="H22" s="20"/>
       <c r="I22" s="26"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="29"/>
+      <c r="K22" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23" s="13">
         <v>34</v>
       </c>
@@ -1001,8 +1097,12 @@
       <c r="G23" s="1"/>
       <c r="H23" s="20"/>
       <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="29"/>
+      <c r="K23" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24" s="13">
         <v>35</v>
       </c>
@@ -1012,8 +1112,12 @@
       <c r="G24" s="1"/>
       <c r="H24" s="20"/>
       <c r="I24" s="26"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="29"/>
+      <c r="K24" s="11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="13">
         <v>36</v>
       </c>
@@ -1023,8 +1127,14 @@
       <c r="G25" s="1"/>
       <c r="H25" s="20"/>
       <c r="I25" s="26"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="13">
         <v>37</v>
       </c>
@@ -1034,8 +1144,12 @@
       <c r="G26" s="1"/>
       <c r="H26" s="20"/>
       <c r="I26" s="26"/>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="11"/>
+      <c r="K26" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27" s="13">
         <v>38</v>
       </c>
@@ -1045,8 +1159,12 @@
       <c r="G27" s="1"/>
       <c r="H27" s="20"/>
       <c r="I27" s="26"/>
-    </row>
-    <row r="28" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="11"/>
+      <c r="K27" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="14">
         <v>39</v>
       </c>
@@ -1056,6 +1174,10 @@
       <c r="G28" s="5"/>
       <c r="H28" s="21"/>
       <c r="I28" s="27"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commit 2019-06-22 kl. 19:28
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -57,13 +57,13 @@
     <t>Juli</t>
   </si>
   <si>
-    <t>Augisti</t>
-  </si>
-  <si>
     <t>September</t>
   </si>
   <si>
     <t>Date Friday</t>
+  </si>
+  <si>
+    <t>Augusti</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -733,7 +733,7 @@
   <dimension ref="C1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,11 +790,11 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
@@ -875,12 +875,14 @@
       <c r="C9" s="13">
         <v>20</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="26"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="26">
+        <v>5</v>
+      </c>
       <c r="J9" s="29"/>
       <c r="K9" s="11">
         <v>17</v>
@@ -890,12 +892,14 @@
       <c r="C10" s="13">
         <v>21</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="26"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="26">
+        <v>5</v>
+      </c>
       <c r="J10" s="29"/>
       <c r="K10" s="11">
         <v>24</v>
@@ -906,11 +910,13 @@
         <v>22</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="26"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="26">
+        <v>5</v>
+      </c>
       <c r="J11" s="29"/>
       <c r="K11" s="11">
         <v>31</v>
@@ -920,12 +926,14 @@
       <c r="C12" s="13">
         <v>23</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="26"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="26">
+        <v>5</v>
+      </c>
       <c r="J12" s="29" t="s">
         <v>10</v>
       </c>
@@ -937,12 +945,14 @@
       <c r="C13" s="13">
         <v>24</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="26"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="26">
+        <v>5</v>
+      </c>
       <c r="J13" s="29"/>
       <c r="K13" s="11">
         <v>14</v>
@@ -952,12 +962,14 @@
       <c r="C14" s="13">
         <v>25</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="26"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="26">
+        <v>5</v>
+      </c>
       <c r="J14" s="29"/>
       <c r="K14" s="11">
         <v>21</v>
@@ -1051,7 +1063,7 @@
       <c r="H20" s="20"/>
       <c r="I20" s="26"/>
       <c r="J20" s="29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K20" s="11">
         <v>1</v>
@@ -1128,7 +1140,7 @@
       <c r="H25" s="20"/>
       <c r="I25" s="26"/>
       <c r="J25" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K25" s="11">
         <v>6</v>

</xml_diff>

<commit_message>
Commit 2019-06-24 kl. 09:13
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Week</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Augusti</t>
+  </si>
+  <si>
+    <t>Lön</t>
   </si>
 </sst>
 </file>
@@ -790,11 +793,11 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
@@ -915,7 +918,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J11" s="29"/>
       <c r="K11" s="11">
@@ -980,7 +983,9 @@
         <v>26</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="20"/>
@@ -1044,7 +1049,9 @@
       <c r="D19" s="8"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H19" s="20"/>
       <c r="I19" s="26"/>
       <c r="J19" s="29"/>
@@ -1107,7 +1114,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="20"/>
+      <c r="H23" s="20" t="s">
+        <v>15</v>
+      </c>
       <c r="I23" s="26"/>
       <c r="J23" s="29"/>
       <c r="K23" s="11">
@@ -1182,7 +1191,9 @@
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="21"/>
       <c r="I28" s="27"/>

</xml_diff>

<commit_message>
Commit 2019-06-27 kl. 09:33
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -725,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -736,7 +736,7 @@
   <dimension ref="C1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,11 +793,11 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="3:12" x14ac:dyDescent="0.25">
@@ -982,14 +982,16 @@
       <c r="C15" s="13">
         <v>26</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="1"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="26"/>
+      <c r="I15" s="26">
+        <v>3</v>
+      </c>
       <c r="J15" s="29"/>
       <c r="K15" s="11">
         <v>28</v>

</xml_diff>

<commit_message>
Commit 2019-07-05 kl. 09:30
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Week</t>
   </si>
@@ -67,13 +67,16 @@
   </si>
   <si>
     <t>Lön</t>
+  </si>
+  <si>
+    <t>% done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +86,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -360,10 +370,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -414,9 +425,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -733,11 +749,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:L28"/>
+  <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -747,10 +761,11 @@
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
@@ -778,8 +793,11 @@
       <c r="L2" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C3" s="12">
         <v>14</v>
       </c>
@@ -793,14 +811,18 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="M3" s="31">
+        <f>L3/125</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="13">
         <v>15</v>
       </c>
@@ -813,7 +835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C5" s="13">
         <v>16</v>
       </c>
@@ -826,7 +848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C6" s="13">
         <v>17</v>
       </c>
@@ -839,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C7" s="13">
         <v>18</v>
       </c>
@@ -855,7 +877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C8" s="13">
         <v>19</v>
       </c>
@@ -874,7 +896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9" s="13">
         <v>20</v>
       </c>
@@ -891,7 +913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C10" s="13">
         <v>21</v>
       </c>
@@ -908,7 +930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C11" s="13">
         <v>22</v>
       </c>
@@ -925,7 +947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C12" s="13">
         <v>23</v>
       </c>
@@ -944,7 +966,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="13">
         <v>24</v>
       </c>
@@ -961,7 +983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C14" s="13">
         <v>25</v>
       </c>
@@ -978,7 +1000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15" s="13">
         <v>26</v>
       </c>
@@ -987,26 +1009,28 @@
         <v>15</v>
       </c>
       <c r="F15" s="17"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="20"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
       <c r="I15" s="26">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J15" s="29"/>
       <c r="K15" s="11">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C16" s="13">
         <v>27</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="26"/>
+      <c r="I16" s="26">
+        <v>4</v>
+      </c>
       <c r="J16" s="29" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Commit 2019-07-05 kl. 18:33
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,7 +751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -811,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.52</v>
+        <v>0.52800000000000002</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1027,9 +1029,9 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="20"/>
+      <c r="H16" s="17"/>
       <c r="I16" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J16" s="29" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Commit 2019-07-21 kl. 21:57
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.52800000000000002</v>
+        <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1044,12 +1044,14 @@
       <c r="C17" s="13">
         <v>28</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="26"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="26">
+        <v>5</v>
+      </c>
       <c r="J17" s="29"/>
       <c r="K17" s="11">
         <v>12</v>
@@ -1059,12 +1061,14 @@
       <c r="C18" s="13">
         <v>29</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="26"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="26">
+        <v>5</v>
+      </c>
       <c r="J18" s="29"/>
       <c r="K18" s="11">
         <v>19</v>

</xml_diff>

<commit_message>
Commit 2019-07-25 kl. 09:12
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,9 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -813,15 +811,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.60799999999999998</v>
+        <v>0.63200000000000001</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1078,14 +1076,16 @@
       <c r="C19" s="13">
         <v>30</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="20"/>
-      <c r="I19" s="26"/>
+      <c r="I19" s="26">
+        <v>3</v>
+      </c>
       <c r="J19" s="29"/>
       <c r="K19" s="11">
         <v>26</v>

</xml_diff>

<commit_message>
Commit 2019-07-26 kl. 09:14
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,7 +751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -811,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.63200000000000001</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1079,12 +1081,12 @@
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="17" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J19" s="29"/>
       <c r="K19" s="11">

</xml_diff>

<commit_message>
Commit 2019-08-01 kl. 09:24
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.64</v>
+        <v>0.67200000000000004</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1084,9 +1084,9 @@
       <c r="G19" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="20"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J19" s="29"/>
       <c r="K19" s="11">
@@ -1097,12 +1097,14 @@
       <c r="C20" s="13">
         <v>31</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="1"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="26"/>
+      <c r="I20" s="26">
+        <v>3</v>
+      </c>
       <c r="J20" s="29" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Commit 2019-08-02 kl. 09:09
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.67200000000000004</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1100,16 +1100,16 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="20"/>
       <c r="I20" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
@@ -1124,7 +1124,7 @@
       <c r="I21" s="26"/>
       <c r="J21" s="29"/>
       <c r="K21" s="11">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
       <c r="I22" s="26"/>
       <c r="J22" s="29"/>
       <c r="K22" s="11">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       <c r="I23" s="26"/>
       <c r="J23" s="29"/>
       <c r="K23" s="11">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
       <c r="I24" s="26"/>
       <c r="J24" s="29"/>
       <c r="K24" s="11">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 2019-08-02 kl. 17:35
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.68</v>
+        <v>0.68799999999999994</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1101,9 +1101,9 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="20"/>
+      <c r="H20" s="17"/>
       <c r="I20" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J20" s="29" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Commit 2019-08-08 kl. 09:15
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,9 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -813,15 +811,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.68799999999999994</v>
+        <v>0.71199999999999997</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1116,12 +1114,14 @@
       <c r="C21" s="13">
         <v>32</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="1"/>
       <c r="H21" s="20"/>
-      <c r="I21" s="26"/>
+      <c r="I21" s="26">
+        <v>3</v>
+      </c>
       <c r="J21" s="29"/>
       <c r="K21" s="11">
         <v>9</v>

</xml_diff>

<commit_message>
Commit 2019-08-09 kl. 09:20
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -751,7 +751,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -811,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.71199999999999997</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1117,10 +1119,10 @@
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="17"/>
       <c r="H21" s="20"/>
       <c r="I21" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="11">

</xml_diff>

<commit_message>
Commit 2019-08-11 kl. 00:00
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.72</v>
+        <v>0.72799999999999998</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1120,9 +1120,9 @@
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="20"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="11">

</xml_diff>

<commit_message>
Commit 2019-08-14 kl. 09:22
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.72799999999999998</v>
+        <v>0.74399999999999999</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1133,12 +1133,14 @@
       <c r="C22" s="13">
         <v>33</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="26"/>
+      <c r="I22" s="26">
+        <v>2</v>
+      </c>
       <c r="J22" s="29"/>
       <c r="K22" s="11">
         <v>16</v>

</xml_diff>

<commit_message>
Commit 2019-08-16 kl. 09:21
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.74399999999999999</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1135,11 +1135,11 @@
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="20"/>
       <c r="I22" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J22" s="29"/>
       <c r="K22" s="11">

</xml_diff>

<commit_message>
Commit 2019-08-19 kl. 08:59
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.76</v>
+        <v>0.76800000000000002</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1137,9 +1137,9 @@
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="20"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J22" s="29"/>
       <c r="K22" s="11">

</xml_diff>

<commit_message>
Commit 2019-08-23 kl. 09:18
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.76800000000000002</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1150,14 +1150,16 @@
       <c r="C23" s="13">
         <v>34</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
       <c r="H23" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="26"/>
+      <c r="I23" s="26">
+        <v>4</v>
+      </c>
       <c r="J23" s="29"/>
       <c r="K23" s="11">
         <v>23</v>

</xml_diff>

<commit_message>
Commit 2019-09-10 kl. 20:22
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.8</v>
+        <v>0.89600000000000002</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1154,11 +1154,11 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="18" t="s">
         <v>15</v>
       </c>
       <c r="I23" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="11">
@@ -1170,11 +1170,13 @@
         <v>35</v>
       </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="26"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="26">
+        <v>4</v>
+      </c>
       <c r="J24" s="29"/>
       <c r="K24" s="11">
         <v>30</v>
@@ -1184,12 +1186,14 @@
       <c r="C25" s="13">
         <v>36</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="26"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="26">
+        <v>5</v>
+      </c>
       <c r="J25" s="29" t="s">
         <v>12</v>
       </c>
@@ -1201,12 +1205,14 @@
       <c r="C26" s="13">
         <v>37</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="26"/>
+      <c r="I26" s="26">
+        <v>2</v>
+      </c>
       <c r="J26" s="11"/>
       <c r="K26" s="11">
         <v>13</v>

</xml_diff>

<commit_message>
Commit 2019-09-13 kl. 09:22
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.89600000000000002</v>
+        <v>0.91200000000000003</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1207,11 +1207,11 @@
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="20"/>
       <c r="I26" s="26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J26" s="11"/>
       <c r="K26" s="11">

</xml_diff>

<commit_message>
Commit 2019-09-16 kl. 09:30
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -741,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,7 +752,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,15 +813,15 @@
       </c>
       <c r="K3" s="7">
         <f>125-L3</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3" s="7">
         <f>SUM(I3:I28)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M3" s="31">
         <f>L3/125</f>
-        <v>0.91200000000000003</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -1209,9 +1209,9 @@
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
-      <c r="H26" s="20"/>
+      <c r="H26" s="17"/>
       <c r="I26" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J26" s="11"/>
       <c r="K26" s="11">

</xml_diff>

<commit_message>
Commit 2019-09-21 kl. 22:09
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -374,9 +374,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -385,7 +384,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -407,7 +405,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -741,7 +738,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -752,12 +749,12 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="9" customWidth="1"/>
     <col min="4" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
@@ -768,485 +765,487 @@
   <sheetData>
     <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="27" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>14</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="25">
-        <v>5</v>
-      </c>
-      <c r="K3" s="7">
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22">
+        <v>5</v>
+      </c>
+      <c r="K3" s="6">
         <f>125-L3</f>
+        <v>5</v>
+      </c>
+      <c r="L3" s="6">
+        <f>SUM(I3:I28)</f>
+        <v>120</v>
+      </c>
+      <c r="M3" s="28">
+        <f>L3/125</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="11">
+        <v>15</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="11">
+        <v>16</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="11">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="11">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="23">
+        <v>5</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="11">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="23">
+        <v>4</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="9">
         <v>10</v>
       </c>
-      <c r="L3" s="7">
-        <f>SUM(I3:I28)</f>
-        <v>115</v>
-      </c>
-      <c r="M3" s="31">
-        <f>L3/125</f>
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="13">
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="11">
+        <v>20</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="23">
+        <v>5</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="11">
+        <v>21</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="23">
+        <v>5</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C11" s="11">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="23">
+        <v>4</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="11">
+        <v>23</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="23">
+        <v>5</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C13" s="11">
+        <v>24</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="23">
+        <v>5</v>
+      </c>
+      <c r="J13" s="26"/>
+      <c r="K13" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C14" s="11">
+        <v>25</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="23">
+        <v>5</v>
+      </c>
+      <c r="J14" s="26"/>
+      <c r="K14" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="13">
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="23">
+        <v>5</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="K15" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="11">
+        <v>27</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="23">
+        <v>5</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="11">
+        <v>28</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="23">
+        <v>5</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="11">
+        <v>29</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="23">
+        <v>5</v>
+      </c>
+      <c r="J18" s="26"/>
+      <c r="K18" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="11">
+        <v>30</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="23">
+        <v>5</v>
+      </c>
+      <c r="J19" s="26"/>
+      <c r="K19" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="11">
+        <v>31</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="23">
+        <v>5</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="11">
+        <v>32</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="23">
+        <v>5</v>
+      </c>
+      <c r="J21" s="26"/>
+      <c r="K21" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="11">
+        <v>33</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="23">
+        <v>5</v>
+      </c>
+      <c r="J22" s="26"/>
+      <c r="K22" s="9">
         <v>16</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="26">
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="11">
+        <v>34</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="23">
+        <v>5</v>
+      </c>
+      <c r="J23" s="26"/>
+      <c r="K23" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="11">
+        <v>35</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="23">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="13">
-        <v>17</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="13">
-        <v>18</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="26">
-        <v>5</v>
-      </c>
-      <c r="K7" s="28" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="11">
+        <v>36</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="23">
+        <v>5</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="11">
+        <v>37</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="23">
+        <v>5</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="13">
-        <v>19</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="26">
-        <v>4</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="13">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="11">
+        <v>38</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="23">
+        <v>5</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9">
         <v>20</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="26">
-        <v>5</v>
-      </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="11">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="13">
-        <v>21</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="26">
-        <v>5</v>
-      </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="13">
-        <v>22</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="26">
-        <v>4</v>
-      </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="11">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="13">
-        <v>23</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="26">
-        <v>5</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="13">
-        <v>24</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="26">
-        <v>5</v>
-      </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="13">
-        <v>25</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="26">
-        <v>5</v>
-      </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="11">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="13">
-        <v>26</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17" t="s">
+    </row>
+    <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="12">
+        <v>39</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="26">
-        <v>5</v>
-      </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="11">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="13">
-        <v>27</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="26">
-        <v>5</v>
-      </c>
-      <c r="J16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="13">
-        <v>28</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="26">
-        <v>5</v>
-      </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="13">
-        <v>29</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="26">
-        <v>5</v>
-      </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="11">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="13">
-        <v>30</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="26">
-        <v>5</v>
-      </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="11">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="13">
-        <v>31</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="26">
-        <v>5</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="13">
-        <v>32</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="26">
-        <v>5</v>
-      </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="13">
-        <v>33</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="26">
-        <v>5</v>
-      </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="13">
-        <v>34</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="26">
-        <v>5</v>
-      </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="11">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="13">
-        <v>35</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="26">
-        <v>4</v>
-      </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="13">
-        <v>36</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="26">
-        <v>5</v>
-      </c>
-      <c r="J25" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="13">
-        <v>37</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="26">
-        <v>5</v>
-      </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="13">
-        <v>38</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="14">
-        <v>39</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11">
+      <c r="G28" s="4"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 2019-09-26 kl. 09:20
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -126,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -276,21 +276,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -385,7 +370,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,13 +387,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,6 +410,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -749,12 +734,12 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="8" customWidth="1"/>
     <col min="4" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
@@ -765,7 +750,7 @@
   <sheetData>
     <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -792,460 +777,462 @@
       <c r="L2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>14</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22">
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21">
         <v>5</v>
       </c>
       <c r="K3" s="6">
         <f>125-L3</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L3" s="6">
         <f>SUM(I3:I28)</f>
-        <v>120</v>
-      </c>
-      <c r="M3" s="28">
+        <v>123</v>
+      </c>
+      <c r="M3" s="27">
         <f>L3/125</f>
-        <v>0.96</v>
+        <v>0.98399999999999999</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>15</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="23">
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>16</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="23">
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>17</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="23">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>18</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="23">
-        <v>5</v>
-      </c>
-      <c r="K7" s="25" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="22">
+        <v>5</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>19</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="23">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="22">
         <v>4</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>20</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="23">
-        <v>5</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="9">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="22">
+        <v>5</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="8">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>21</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="23">
-        <v>5</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="9">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="22">
+        <v>5</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="8">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>22</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="23">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="22">
         <v>4</v>
       </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="9">
+      <c r="J11" s="25"/>
+      <c r="K11" s="8">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>23</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="23">
-        <v>5</v>
-      </c>
-      <c r="J12" s="26" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="22">
+        <v>5</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>24</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="23">
-        <v>5</v>
-      </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="9">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="22">
+        <v>5</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>25</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="23">
-        <v>5</v>
-      </c>
-      <c r="J14" s="26"/>
-      <c r="K14" s="9">
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="22">
+        <v>5</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="8">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>26</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="23">
-        <v>5</v>
-      </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="9">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="22">
+        <v>5</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="8">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>27</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="23">
-        <v>5</v>
-      </c>
-      <c r="J16" s="26" t="s">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="22">
+        <v>5</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>28</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="23">
-        <v>5</v>
-      </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="9">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="22">
+        <v>5</v>
+      </c>
+      <c r="J17" s="25"/>
+      <c r="K17" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>29</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="23">
-        <v>5</v>
-      </c>
-      <c r="J18" s="26"/>
-      <c r="K18" s="9">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="22">
+        <v>5</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="8">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>30</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15" t="s">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="23">
-        <v>5</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="9">
+      <c r="H19" s="14"/>
+      <c r="I19" s="22">
+        <v>5</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="8">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>31</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="23">
-        <v>5</v>
-      </c>
-      <c r="J20" s="26" t="s">
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="22">
+        <v>5</v>
+      </c>
+      <c r="J20" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>32</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="23">
-        <v>5</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="9">
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="22">
+        <v>5</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>33</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="23">
-        <v>5</v>
-      </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="9">
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="22">
+        <v>5</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="8">
         <v>16</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>34</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16" t="s">
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="23">
-        <v>5</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="9">
+      <c r="I23" s="22">
+        <v>5</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="8">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>35</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="23">
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="22">
         <v>4</v>
       </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="9">
+      <c r="J24" s="25"/>
+      <c r="K24" s="8">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>36</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="23">
-        <v>5</v>
-      </c>
-      <c r="J25" s="26" t="s">
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="22">
+        <v>5</v>
+      </c>
+      <c r="J25" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>37</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="23">
-        <v>5</v>
-      </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="22">
+        <v>5</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>38</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="23">
-        <v>5</v>
-      </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="22">
+        <v>5</v>
+      </c>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="12">
+      <c r="C28" s="11">
         <v>39</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9">
+      <c r="H28" s="17"/>
+      <c r="I28" s="23">
+        <v>3</v>
+      </c>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 2019-09-27 kl. 09:26
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -359,12 +359,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -723,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -734,12 +733,12 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="6.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="7" customWidth="1"/>
     <col min="4" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
@@ -750,7 +749,7 @@
   <sheetData>
     <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -771,468 +770,468 @@
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>14</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21">
-        <v>5</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20">
+        <v>5</v>
+      </c>
+      <c r="K3" s="5">
         <f>125-L3</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
+        <f>SUM(I3:I28)</f>
+        <v>124</v>
+      </c>
+      <c r="M3" s="26">
+        <f>L3/125</f>
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C4" s="9">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C5" s="9">
+        <v>16</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C7" s="9">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="21">
+        <v>5</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C8" s="9">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="21">
+        <v>4</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="21">
+        <v>5</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
+        <v>21</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="21">
+        <v>5</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
+        <v>22</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="21">
+        <v>4</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
+        <v>23</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="21">
+        <v>5</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
+        <v>24</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="21">
+        <v>5</v>
+      </c>
+      <c r="J13" s="24"/>
+      <c r="K13" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C14" s="9">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="21">
+        <v>5</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C15" s="9">
+        <v>26</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="21">
+        <v>5</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="9">
+        <v>27</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="21">
+        <v>5</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="9">
+        <v>28</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="21">
+        <v>5</v>
+      </c>
+      <c r="J17" s="24"/>
+      <c r="K17" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="9">
+        <v>29</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="21">
+        <v>5</v>
+      </c>
+      <c r="J18" s="24"/>
+      <c r="K18" s="7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="9">
+        <v>30</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="21">
+        <v>5</v>
+      </c>
+      <c r="J19" s="24"/>
+      <c r="K19" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="9">
+        <v>31</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="21">
+        <v>5</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="7">
         <v>2</v>
       </c>
-      <c r="L3" s="6">
-        <f>SUM(I3:I28)</f>
-        <v>123</v>
-      </c>
-      <c r="M3" s="27">
-        <f>L3/125</f>
-        <v>0.98399999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="10">
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="9">
+        <v>32</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="21">
+        <v>5</v>
+      </c>
+      <c r="J21" s="24"/>
+      <c r="K21" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="9">
+        <v>33</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="21">
+        <v>5</v>
+      </c>
+      <c r="J22" s="24"/>
+      <c r="K22" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="9">
+        <v>34</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="10">
-        <v>16</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="22">
+      <c r="I23" s="21">
+        <v>5</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="9">
+        <v>35</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="21">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="10">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="22">
+      <c r="J24" s="24"/>
+      <c r="K24" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="9">
+        <v>36</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="21">
+        <v>5</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="9">
+        <v>37</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="21">
+        <v>5</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="9">
+        <v>38</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="21">
+        <v>5</v>
+      </c>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="10">
+        <v>39</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="22">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="10">
-        <v>18</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="22">
-        <v>5</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="10">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="22">
-        <v>4</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="10">
-        <v>20</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="22">
-        <v>5</v>
-      </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="8">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="10">
-        <v>21</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="22">
-        <v>5</v>
-      </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="8">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="10">
-        <v>22</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="22">
-        <v>4</v>
-      </c>
-      <c r="J11" s="25"/>
-      <c r="K11" s="8">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="10">
-        <v>23</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="22">
-        <v>5</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="10">
-        <v>24</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="22">
-        <v>5</v>
-      </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C14" s="10">
-        <v>25</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="22">
-        <v>5</v>
-      </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="10">
-        <v>26</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="22">
-        <v>5</v>
-      </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="8">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="10">
-        <v>27</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="22">
-        <v>5</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="10">
-        <v>28</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="22">
-        <v>5</v>
-      </c>
-      <c r="J17" s="25"/>
-      <c r="K17" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="10">
-        <v>29</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="22">
-        <v>5</v>
-      </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="8">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="10">
-        <v>30</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="22">
-        <v>5</v>
-      </c>
-      <c r="J19" s="25"/>
-      <c r="K19" s="8">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="10">
-        <v>31</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="22">
-        <v>5</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="10">
-        <v>32</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="22">
-        <v>5</v>
-      </c>
-      <c r="J21" s="25"/>
-      <c r="K21" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="10">
-        <v>33</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="22">
-        <v>5</v>
-      </c>
-      <c r="J22" s="25"/>
-      <c r="K22" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="10">
-        <v>34</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="22">
-        <v>5</v>
-      </c>
-      <c r="J23" s="25"/>
-      <c r="K23" s="8">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="10">
-        <v>35</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="22">
-        <v>4</v>
-      </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="10">
-        <v>36</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="22">
-        <v>5</v>
-      </c>
-      <c r="J25" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="10">
-        <v>37</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="22">
-        <v>5</v>
-      </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="10">
-        <v>38</v>
-      </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="22">
-        <v>5</v>
-      </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="11">
-        <v>39</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="23">
-        <v>3</v>
-      </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8">
+      <c r="J28" s="7"/>
+      <c r="K28" s="7">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commit 2019-09-27 kl. 17:31
</commit_message>
<xml_diff>
--- a/Administration/Fixzone.xlsx
+++ b/Administration/Fixzone.xlsx
@@ -126,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -281,11 +281,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -294,26 +296,15 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -324,7 +315,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -332,24 +325,58 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -359,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -386,13 +413,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -410,6 +431,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +750,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -733,7 +761,7 @@
   <dimension ref="C1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +804,7 @@
       <c r="L2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -784,25 +812,25 @@
       <c r="C3" s="8">
         <v>14</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="14">
         <v>5</v>
       </c>
       <c r="K3" s="5">
         <f>125-L3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="5">
         <f>SUM(I3:I28)</f>
-        <v>124</v>
-      </c>
-      <c r="M3" s="26">
+        <v>125</v>
+      </c>
+      <c r="M3" s="20">
         <f>L3/125</f>
-        <v>0.99199999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
@@ -813,8 +841,8 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="21">
+      <c r="H4" s="25"/>
+      <c r="I4" s="15">
         <v>5</v>
       </c>
     </row>
@@ -826,8 +854,8 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="21">
+      <c r="H5" s="26"/>
+      <c r="I5" s="15">
         <v>4</v>
       </c>
     </row>
@@ -839,8 +867,8 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="21">
+      <c r="H6" s="25"/>
+      <c r="I6" s="15">
         <v>4</v>
       </c>
     </row>
@@ -852,11 +880,11 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="21">
-        <v>5</v>
-      </c>
-      <c r="K7" s="23" t="s">
+      <c r="H7" s="25"/>
+      <c r="I7" s="15">
+        <v>5</v>
+      </c>
+      <c r="K7" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -868,11 +896,11 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="21">
+      <c r="H8" s="25"/>
+      <c r="I8" s="15">
         <v>4</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="18" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="7">
@@ -883,15 +911,15 @@
       <c r="C9" s="9">
         <v>20</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="21">
-        <v>5</v>
-      </c>
-      <c r="J9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="15">
+        <v>5</v>
+      </c>
+      <c r="J9" s="18"/>
       <c r="K9" s="7">
         <v>17</v>
       </c>
@@ -900,15 +928,15 @@
       <c r="C10" s="9">
         <v>21</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="21">
-        <v>5</v>
-      </c>
-      <c r="J10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="15">
+        <v>5</v>
+      </c>
+      <c r="J10" s="18"/>
       <c r="K10" s="7">
         <v>24</v>
       </c>
@@ -921,11 +949,11 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="21">
+      <c r="H11" s="25"/>
+      <c r="I11" s="15">
         <v>4</v>
       </c>
-      <c r="J11" s="24"/>
+      <c r="J11" s="18"/>
       <c r="K11" s="7">
         <v>31</v>
       </c>
@@ -934,15 +962,15 @@
       <c r="C12" s="9">
         <v>23</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="21">
-        <v>5</v>
-      </c>
-      <c r="J12" s="24" t="s">
+      <c r="H12" s="25"/>
+      <c r="I12" s="15">
+        <v>5</v>
+      </c>
+      <c r="J12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="7">
@@ -953,15 +981,15 @@
       <c r="C13" s="9">
         <v>24</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="21">
-        <v>5</v>
-      </c>
-      <c r="J13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="15">
+        <v>5</v>
+      </c>
+      <c r="J13" s="18"/>
       <c r="K13" s="7">
         <v>14</v>
       </c>
@@ -970,15 +998,15 @@
       <c r="C14" s="9">
         <v>25</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="21">
-        <v>5</v>
-      </c>
-      <c r="J14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="15">
+        <v>5</v>
+      </c>
+      <c r="J14" s="18"/>
       <c r="K14" s="7">
         <v>21</v>
       </c>
@@ -987,17 +1015,17 @@
       <c r="C15" s="9">
         <v>26</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="21">
-        <v>5</v>
-      </c>
-      <c r="J15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="15">
+        <v>5</v>
+      </c>
+      <c r="J15" s="18"/>
       <c r="K15" s="7">
         <v>28</v>
       </c>
@@ -1006,15 +1034,15 @@
       <c r="C16" s="9">
         <v>27</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="21">
-        <v>5</v>
-      </c>
-      <c r="J16" s="24" t="s">
+      <c r="H16" s="25"/>
+      <c r="I16" s="15">
+        <v>5</v>
+      </c>
+      <c r="J16" s="18" t="s">
         <v>11</v>
       </c>
       <c r="K16" s="7">
@@ -1025,15 +1053,15 @@
       <c r="C17" s="9">
         <v>28</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="21">
-        <v>5</v>
-      </c>
-      <c r="J17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="15">
+        <v>5</v>
+      </c>
+      <c r="J17" s="18"/>
       <c r="K17" s="7">
         <v>12</v>
       </c>
@@ -1042,15 +1070,15 @@
       <c r="C18" s="9">
         <v>29</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="21">
-        <v>5</v>
-      </c>
-      <c r="J18" s="24"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="15">
+        <v>5</v>
+      </c>
+      <c r="J18" s="18"/>
       <c r="K18" s="7">
         <v>19</v>
       </c>
@@ -1059,17 +1087,17 @@
       <c r="C19" s="9">
         <v>30</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="21">
-        <v>5</v>
-      </c>
-      <c r="J19" s="24"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="15">
+        <v>5</v>
+      </c>
+      <c r="J19" s="18"/>
       <c r="K19" s="7">
         <v>26</v>
       </c>
@@ -1078,15 +1106,15 @@
       <c r="C20" s="9">
         <v>31</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="21">
-        <v>5</v>
-      </c>
-      <c r="J20" s="24" t="s">
+      <c r="H20" s="25"/>
+      <c r="I20" s="15">
+        <v>5</v>
+      </c>
+      <c r="J20" s="18" t="s">
         <v>14</v>
       </c>
       <c r="K20" s="7">
@@ -1097,15 +1125,15 @@
       <c r="C21" s="9">
         <v>32</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="21">
-        <v>5</v>
-      </c>
-      <c r="J21" s="24"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="15">
+        <v>5</v>
+      </c>
+      <c r="J21" s="18"/>
       <c r="K21" s="7">
         <v>9</v>
       </c>
@@ -1114,15 +1142,15 @@
       <c r="C22" s="9">
         <v>33</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="21">
-        <v>5</v>
-      </c>
-      <c r="J22" s="24"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="15">
+        <v>5</v>
+      </c>
+      <c r="J22" s="18"/>
       <c r="K22" s="7">
         <v>16</v>
       </c>
@@ -1131,17 +1159,17 @@
       <c r="C23" s="9">
         <v>34</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="21">
-        <v>5</v>
-      </c>
-      <c r="J23" s="24"/>
+      <c r="I23" s="15">
+        <v>5</v>
+      </c>
+      <c r="J23" s="18"/>
       <c r="K23" s="7">
         <v>23</v>
       </c>
@@ -1154,11 +1182,11 @@
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="21">
+      <c r="H24" s="25"/>
+      <c r="I24" s="15">
         <v>4</v>
       </c>
-      <c r="J24" s="24"/>
+      <c r="J24" s="18"/>
       <c r="K24" s="7">
         <v>30</v>
       </c>
@@ -1167,15 +1195,15 @@
       <c r="C25" s="9">
         <v>36</v>
       </c>
-      <c r="D25" s="13"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="21">
-        <v>5</v>
-      </c>
-      <c r="J25" s="24" t="s">
+      <c r="H25" s="25"/>
+      <c r="I25" s="15">
+        <v>5</v>
+      </c>
+      <c r="J25" s="18" t="s">
         <v>12</v>
       </c>
       <c r="K25" s="7">
@@ -1186,12 +1214,12 @@
       <c r="C26" s="9">
         <v>37</v>
       </c>
-      <c r="D26" s="13"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="21">
+      <c r="H26" s="25"/>
+      <c r="I26" s="15">
         <v>5</v>
       </c>
       <c r="J26" s="7"/>
@@ -1203,12 +1231,12 @@
       <c r="C27" s="9">
         <v>38</v>
       </c>
-      <c r="D27" s="13"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="21">
+      <c r="H27" s="25"/>
+      <c r="I27" s="15">
         <v>5</v>
       </c>
       <c r="J27" s="7"/>
@@ -1220,15 +1248,15 @@
       <c r="C28" s="10">
         <v>39</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="27" t="s">
+      <c r="D28" s="27"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="13"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="22">
-        <v>4</v>
+      <c r="G28" s="21"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="16">
+        <v>5</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7">

</xml_diff>